<commit_message>
inconsequential update to INQUIRE source data tables
</commit_message>
<xml_diff>
--- a/linkml/source_tables/INQUIRE/BiomarkerList_v2.25_UA - update 24Oct2023 - Cleaned.xlsx
+++ b/linkml/source_tables/INQUIRE/BiomarkerList_v2.25_UA - update 24Oct2023 - Cleaned.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vitoresearch-my.sharepoint.com/personal/dirk_devriendt_ext_vito_be/Documents/Documents/INQUIRE/Data Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vitoresearch-my.sharepoint.com/personal/dirk_devriendt_ext_vito_be/Documents/Documents/git/parco-hbm/linkml/source_tables/INQUIRE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{FE3F32E1-355B-49F4-B2BB-44F808CC1DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBC98C5F-B1C3-48EB-89C6-6FD4388A2957}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{FE3F32E1-355B-49F4-B2BB-44F808CC1DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2CE01ED-7831-432E-9F89-18A2A4952660}"/>
   <bookViews>
-    <workbookView xWindow="-46950" yWindow="-3870" windowWidth="32160" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36000" yWindow="-9405" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="2" r:id="rId1"/>
@@ -6483,7 +6483,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomLeft" activeCell="E478" sqref="E49:E478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>